<commit_message>
User schema designing start
</commit_message>
<xml_diff>
--- a/_dev/DbDesign_10_01.xlsx
+++ b/_dev/DbDesign_10_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Aher\Desktop\Resourse-Guru-master\_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB03AB4B-C1B6-4FEE-9E7B-CA663C5CD825}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E90BF7D-54B4-464E-957A-D84F871ADB24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1241,9 +1241,6 @@
     <t>boolean, default true</t>
   </si>
   <si>
-    <t>Allocations</t>
-  </si>
-  <si>
     <t>details</t>
   </si>
   <si>
@@ -1323,13 +1320,16 @@
   </si>
   <si>
     <t>Project (Done)</t>
+  </si>
+  <si>
+    <t>Schedule</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1389,6 +1389,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1703,7 +1710,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1793,6 +1800,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3210,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8575859F-54CF-4BE3-B577-4CD91349768F}">
   <dimension ref="B1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,7 +3251,7 @@
       <c r="F2" s="33"/>
       <c r="G2" s="34"/>
       <c r="J2" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K2" s="33"/>
       <c r="L2" s="33"/>
@@ -3382,7 +3390,7 @@
         <v>143</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>168</v>
@@ -3490,7 +3498,7 @@
         <v>173</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>151</v>
@@ -3586,7 +3594,7 @@
         <v>8805142092</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K14" s="33"/>
       <c r="L14" s="33"/>
@@ -3668,7 +3676,7 @@
     </row>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>152</v>
@@ -3683,7 +3691,7 @@
         <v>153</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>144</v>
@@ -3835,7 +3843,7 @@
         <v>153</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J22" s="20" t="s">
         <v>190</v>
@@ -3857,7 +3865,7 @@
       </c>
     </row>
     <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="41" t="s">
         <v>137</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -3934,7 +3942,7 @@
     </row>
     <row r="25" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>151</v>
@@ -4009,7 +4017,7 @@
       </c>
     </row>
     <row r="27" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="41" t="s">
         <v>141</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -4086,7 +4094,7 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J29" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>151</v>
@@ -4126,7 +4134,7 @@
     </row>
     <row r="31" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>151</v>
@@ -4167,7 +4175,7 @@
     <row r="33" spans="2:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
@@ -4175,7 +4183,7 @@
       <c r="F34" s="33"/>
       <c r="G34" s="34"/>
       <c r="J34" s="32" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
       <c r="K34" s="33"/>
       <c r="L34" s="33"/>
@@ -4290,13 +4298,13 @@
     </row>
     <row r="40" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>143</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>168</v>
@@ -4305,7 +4313,7 @@
         <v>153</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J40" s="20" t="s">
         <v>190</v>
@@ -4328,7 +4336,7 @@
     </row>
     <row r="41" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>143</v>
@@ -4366,7 +4374,7 @@
     </row>
     <row r="42" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>143</v>
@@ -4404,7 +4412,7 @@
     </row>
     <row r="43" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>143</v>
@@ -4419,7 +4427,7 @@
         <v>153</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J43" s="23" t="s">
         <v>210</v>
@@ -4473,12 +4481,12 @@
         <v>153</v>
       </c>
       <c r="O44" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>151</v>
@@ -4516,7 +4524,7 @@
     </row>
     <row r="46" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>143</v>
@@ -4531,7 +4539,7 @@
         <v>153</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>206</v>
@@ -4549,7 +4557,7 @@
         <v>153</v>
       </c>
       <c r="O46" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -4594,7 +4602,7 @@
     </row>
     <row r="49" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
@@ -4643,7 +4651,7 @@
         <v>153</v>
       </c>
       <c r="O50" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4674,7 +4682,7 @@
     </row>
     <row r="52" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J52" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K52" s="10" t="s">
         <v>143</v>
@@ -4725,7 +4733,7 @@
         <v>153</v>
       </c>
       <c r="O53" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4748,7 +4756,7 @@
         <v>169</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K54" s="10" t="s">
         <v>143</v>
@@ -4763,18 +4771,18 @@
         <v>153</v>
       </c>
       <c r="O54" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>143</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E55" s="10" t="s">
         <v>168</v>
@@ -4783,7 +4791,7 @@
         <v>153</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J55" s="10" t="s">
         <v>139</v>
@@ -4824,7 +4832,7 @@
         <v>182</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K56" s="10" t="s">
         <v>151</v>
@@ -4844,7 +4852,7 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>151</v>
@@ -4877,12 +4885,12 @@
         <v>153</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>143</v>
@@ -4897,7 +4905,7 @@
         <v>153</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J58" s="11" t="s">
         <v>184</v>

</xml_diff>

<commit_message>
UI Modifications and new schemas added
</commit_message>
<xml_diff>
--- a/_dev/DbDesign_10_01.xlsx
+++ b/_dev/DbDesign_10_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Aher\Desktop\Resourse-Guru-master\_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E90BF7D-54B4-464E-957A-D84F871ADB24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4579890-171F-4E06-A3EC-8789490F2DF1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="249">
   <si>
     <t>standard  fetaures</t>
   </si>
@@ -983,12 +983,6 @@
     <t>phone</t>
   </si>
   <si>
-    <t>department</t>
-  </si>
-  <si>
-    <t>jobTitle</t>
-  </si>
-  <si>
     <t>isContractor</t>
   </si>
   <si>
@@ -1323,6 +1317,27 @@
   </si>
   <si>
     <t>Schedule</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>departmentName</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>jobName</t>
+  </si>
+  <si>
+    <t>depertmentId</t>
+  </si>
+  <si>
+    <t>departmentNameId</t>
+  </si>
+  <si>
+    <t>jobTitleId</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1475,6 +1490,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1710,7 +1737,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1770,6 +1797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,7 +1828,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2770,10 +2800,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2808,10 +2838,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="32"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2838,10 +2868,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="31"/>
+      <c r="B14" s="32"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2878,10 +2908,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="31"/>
+      <c r="B19" s="32"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2964,10 +2994,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="31"/>
+      <c r="B27" s="32"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -3014,10 +3044,10 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="31"/>
+      <c r="B34" s="32"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -3064,10 +3094,10 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="31"/>
+      <c r="B42" s="32"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -3123,10 +3153,10 @@
       </c>
     </row>
     <row r="49" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="31"/>
+      <c r="B49" s="32"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
@@ -3216,10 +3246,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8575859F-54CF-4BE3-B577-4CD91349768F}">
-  <dimension ref="B1:O59"/>
+  <dimension ref="B1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,88 +3272,88 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34"/>
-      <c r="J2" s="32" t="s">
-        <v>240</v>
-      </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
+      <c r="J2" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="37"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="41"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="G6" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="J6" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="M6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="O6" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3331,37 +3361,37 @@
         <v>128</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J7" s="19" t="s">
         <v>128</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -3369,37 +3399,37 @@
         <v>123</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>170</v>
-      </c>
       <c r="J8" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -3407,37 +3437,37 @@
         <v>124</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J9" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,37 +3475,37 @@
         <v>125</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O10" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3483,37 +3513,37 @@
         <v>126</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O11" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3521,57 +3551,57 @@
         <v>127</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J12" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="18" t="s">
         <v>184</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -3579,96 +3609,96 @@
         <v>129</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G14" s="16">
         <v>8805142092</v>
       </c>
-      <c r="J14" s="32" t="s">
-        <v>242</v>
-      </c>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="34"/>
+      <c r="J14" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="35"/>
     </row>
     <row r="15" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>130</v>
+      <c r="B15" s="43" t="s">
+        <v>247</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="J15" s="35"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="37"/>
+        <v>174</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
     </row>
     <row r="16" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>131</v>
+      <c r="B16" s="44" t="s">
+        <v>248</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J16" s="38"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="40"/>
+        <v>175</v>
+      </c>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G17" s="16" t="b">
         <v>0</v>
@@ -3676,265 +3706,265 @@
     </row>
     <row r="18" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F18" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="M18" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G18" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="K18" s="8" t="s">
+      <c r="N18" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="O18" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N18" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J19" s="22" t="s">
         <v>128</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="N22" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="O22" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
-        <v>137</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O24" s="24">
         <v>44392</v>
@@ -3942,37 +3972,37 @@
     </row>
     <row r="25" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O25" s="24">
         <v>44392</v>
@@ -3980,75 +4010,75 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O26" s="24">
         <v>44392</v>
       </c>
     </row>
     <row r="27" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="41" t="s">
-        <v>141</v>
+      <c r="B27" s="31" t="s">
+        <v>139</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G27" s="16">
         <v>7</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O27" s="24">
         <v>44392</v>
@@ -4056,37 +4086,37 @@
     </row>
     <row r="28" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G28" s="17" t="b">
         <v>1</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O28" s="24">
         <v>44392</v>
@@ -4094,19 +4124,19 @@
     </row>
     <row r="29" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J29" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O29" s="24">
         <v>44392</v>
@@ -4114,148 +4144,148 @@
     </row>
     <row r="30" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J30" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O30" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J32" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O32" s="18" t="s">
         <v>184</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="L32" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="M32" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="N32" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="O32" s="18" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="32" t="s">
-        <v>238</v>
-      </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="34"/>
-      <c r="J34" s="32" t="s">
-        <v>243</v>
-      </c>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="34"/>
+      <c r="B34" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35"/>
+      <c r="J34" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="35"/>
     </row>
     <row r="35" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="37"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="37"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="37"/>
+      <c r="O35" s="38"/>
     </row>
     <row r="36" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="40"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="40"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="41"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="41"/>
     </row>
     <row r="37" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="E38" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="G38" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="J38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L38" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="M38" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N38" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="L38" s="8" t="s">
+      <c r="O38" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="O38" s="12" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4263,260 +4293,260 @@
         <v>128</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J39" s="21" t="s">
         <v>128</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O39" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N40" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O40" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O41" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O42" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>229</v>
-      </c>
       <c r="J43" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N43" s="10"/>
       <c r="O43" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J44" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L44" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="K44" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="L44" s="10" t="s">
-        <v>214</v>
-      </c>
       <c r="M44" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O44" s="25" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N45" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O45" s="26">
         <v>44537</v>
@@ -4524,57 +4554,57 @@
     </row>
     <row r="46" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G46" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>230</v>
-      </c>
       <c r="J46" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O46" s="26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J47" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N47" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O47" s="27">
         <v>0</v>
@@ -4582,99 +4612,99 @@
     </row>
     <row r="48" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J48" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N48" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O48" s="27">
         <v>0.85416666666666663</v>
       </c>
     </row>
     <row r="49" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="34"/>
+      <c r="B49" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="35"/>
       <c r="J49" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O49" s="25" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="37"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="38"/>
       <c r="J50" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O50" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="38"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="40"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="41"/>
       <c r="J51" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K51" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="K51" s="10" t="s">
-        <v>215</v>
-      </c>
       <c r="L51" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N51" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O51" s="25" t="b">
         <v>1</v>
@@ -4682,58 +4712,58 @@
     </row>
     <row r="52" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J52" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N52" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O52" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="E53" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="G53" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E53" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="J53" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N53" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O53" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4741,200 +4771,498 @@
         <v>128</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N54" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O54" s="25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O55" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G56" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N56" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G57" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L57" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M57" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="J58" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K58" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L58" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M58" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N58" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O58" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="35"/>
+      <c r="J61" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="K61" s="34"/>
+      <c r="L61" s="34"/>
+      <c r="M61" s="34"/>
+      <c r="N61" s="34"/>
+      <c r="O61" s="35"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="36"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="38"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" s="38"/>
+    </row>
+    <row r="63" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="39"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="41"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="40"/>
+      <c r="L63" s="40"/>
+      <c r="M63" s="40"/>
+      <c r="N63" s="40"/>
+      <c r="O63" s="41"/>
+    </row>
+    <row r="64" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F58" s="11" t="s">
+      <c r="D65" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G58" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="J58" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="K58" s="11" t="s">
+      <c r="F65" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K65" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="L58" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="M58" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="N58" s="11" t="s">
+      <c r="L65" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="M65" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="O58" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="N65" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="O65" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J66" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M66" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="N66" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="O66" s="13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="K67" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L67" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="M67" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N67" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O67" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J68" s="43" t="s">
+        <v>246</v>
+      </c>
+      <c r="K68" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L68" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="M68" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="N68" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="O68" s="14" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K69" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N69" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="O69" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="K70" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L70" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M70" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N70" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="O70" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J71" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="L71" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="M71" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N71" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O71" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="B2:G4"/>
+    <mergeCell ref="J2:O4"/>
+    <mergeCell ref="J61:O63"/>
+    <mergeCell ref="B61:G63"/>
     <mergeCell ref="J14:O16"/>
     <mergeCell ref="B49:G51"/>
     <mergeCell ref="J34:O36"/>
     <mergeCell ref="B34:G36"/>
-    <mergeCell ref="B2:G4"/>
-    <mergeCell ref="J2:O4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G10" r:id="rId1" xr:uid="{F93B7284-25E3-4BDB-8939-6AD744AED942}"/>

</xml_diff>

<commit_message>
Created two new schemas (CRUD completed)
</commit_message>
<xml_diff>
--- a/_dev/DbDesign_10_01.xlsx
+++ b/_dev/DbDesign_10_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Aher\Desktop\Resourse-Guru-master\_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4579890-171F-4E06-A3EC-8789490F2DF1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587A877F-A11B-4FAD-A32B-89B5D33937AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="249">
   <si>
     <t>standard  fetaures</t>
   </si>
@@ -1331,13 +1331,13 @@
     <t>jobName</t>
   </si>
   <si>
-    <t>depertmentId</t>
-  </si>
-  <si>
     <t>departmentNameId</t>
   </si>
   <si>
     <t>jobTitleId</t>
+  </si>
+  <si>
+    <t>departmentId</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1737,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1798,6 +1798,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1828,9 +1834,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2800,10 +2803,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="36"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2838,10 +2841,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="36"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2868,10 +2871,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="36"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2908,10 +2911,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="32"/>
+      <c r="B19" s="36"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2994,10 +2997,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="36"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -3044,10 +3047,10 @@
       </c>
     </row>
     <row r="34" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="32"/>
+      <c r="B34" s="36"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -3094,10 +3097,10 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="36"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -3153,10 +3156,10 @@
       </c>
     </row>
     <row r="49" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="32"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
@@ -3246,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8575859F-54CF-4BE3-B577-4CD91349768F}">
-  <dimension ref="B1:O71"/>
+  <dimension ref="B1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,50 +3275,50 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35"/>
-      <c r="J2" s="33" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="J2" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="35"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="45"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3623,18 +3626,18 @@
       <c r="G14" s="16">
         <v>8805142092</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="35"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
     </row>
     <row r="15" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
-        <v>247</v>
+      <c r="B15" s="33" t="s">
+        <v>246</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>141</v>
@@ -3651,16 +3654,16 @@
       <c r="G15" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="38"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="44" t="s">
-        <v>248</v>
+      <c r="B16" s="34" t="s">
+        <v>247</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>141</v>
@@ -3677,12 +3680,12 @@
       <c r="G16" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="41"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="45"/>
     </row>
     <row r="17" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
@@ -4204,50 +4207,50 @@
     </row>
     <row r="33" spans="2:15" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-      <c r="J34" s="33" t="s">
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="39"/>
+      <c r="J34" s="37" t="s">
         <v>241</v>
       </c>
-      <c r="K34" s="34"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
-      <c r="O34" s="35"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="39"/>
     </row>
     <row r="35" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="38"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="41"/>
+      <c r="O35" s="42"/>
     </row>
     <row r="36" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="41"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="41"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="45"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="45"/>
     </row>
     <row r="37" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4631,14 +4634,14 @@
       </c>
     </row>
     <row r="49" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="35"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="39"/>
       <c r="J49" s="10" t="s">
         <v>209</v>
       </c>
@@ -4659,12 +4662,12 @@
       </c>
     </row>
     <row r="50" spans="2:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="36"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="38"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
       <c r="J50" s="10" t="s">
         <v>132</v>
       </c>
@@ -4685,12 +4688,12 @@
       </c>
     </row>
     <row r="51" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="39"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="41"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="45"/>
       <c r="J51" s="10" t="s">
         <v>211</v>
       </c>
@@ -4959,50 +4962,50 @@
     <row r="59" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="34"/>
-      <c r="G61" s="35"/>
-      <c r="J61" s="33" t="s">
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="38"/>
+      <c r="G61" s="39"/>
+      <c r="J61" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="K61" s="34"/>
-      <c r="L61" s="34"/>
-      <c r="M61" s="34"/>
-      <c r="N61" s="34"/>
-      <c r="O61" s="35"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="38"/>
+      <c r="M61" s="38"/>
+      <c r="N61" s="38"/>
+      <c r="O61" s="39"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="36"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
-      <c r="J62" s="36"/>
-      <c r="K62" s="37"/>
-      <c r="L62" s="37"/>
-      <c r="M62" s="37"/>
-      <c r="N62" s="37"/>
-      <c r="O62" s="38"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="42"/>
+      <c r="J62" s="40"/>
+      <c r="K62" s="41"/>
+      <c r="L62" s="41"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="42"/>
     </row>
     <row r="63" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="39"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="41"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="40"/>
-      <c r="L63" s="40"/>
-      <c r="M63" s="40"/>
-      <c r="N63" s="40"/>
-      <c r="O63" s="41"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="45"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="44"/>
+      <c r="L63" s="44"/>
+      <c r="M63" s="44"/>
+      <c r="N63" s="44"/>
+      <c r="O63" s="45"/>
     </row>
     <row r="64" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5044,7 +5047,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="33" t="s">
         <v>128</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -5062,7 +5065,7 @@
       <c r="G66" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="J66" s="42" t="s">
+      <c r="J66" s="32" t="s">
         <v>128</v>
       </c>
       <c r="K66" s="9" t="s">
@@ -5098,7 +5101,7 @@
         <v>151</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="J67" s="10" t="s">
         <v>245</v>
@@ -5116,7 +5119,7 @@
         <v>151</v>
       </c>
       <c r="O67" s="14" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5138,8 +5141,8 @@
       <c r="G68" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="J68" s="43" t="s">
-        <v>246</v>
+      <c r="J68" s="33" t="s">
+        <v>248</v>
       </c>
       <c r="K68" s="10" t="s">
         <v>141</v>
@@ -5154,26 +5157,26 @@
         <v>151</v>
       </c>
       <c r="O68" s="14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="G69" s="14" t="s">
+      <c r="D69" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G69" s="11" t="s">
         <v>180</v>
       </c>
       <c r="J69" s="10" t="s">
@@ -5196,61 +5199,23 @@
       </c>
     </row>
     <row r="70" spans="2:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="E70" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="J70" s="10" t="s">
+      <c r="J70" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="K70" s="10" t="s">
+      <c r="K70" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="L70" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="M70" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="N70" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="O70" s="14" t="s">
+      <c r="L70" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="M70" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="N70" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="O70" s="35" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="71" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J71" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="K71" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="L71" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="M71" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="N71" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="O71" s="17" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sidenav opening reolved and create user start
</commit_message>
<xml_diff>
--- a/_dev/DbDesign_10_01.xlsx
+++ b/_dev/DbDesign_10_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Aher\Desktop\Resourse-Guru-master\_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587A877F-A11B-4FAD-A32B-89B5D33937AD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57DE727-C2C4-4DEB-80E4-3402AA0BB044}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3251,8 +3251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8575859F-54CF-4BE3-B577-4CD91349768F}">
   <dimension ref="B1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>